<commit_message>
export to excel fixed
</commit_message>
<xml_diff>
--- a/files/Cunipic.xlsx
+++ b/files/Cunipic.xlsx
@@ -698,23 +698,23 @@
       </c>
       <c r="R3" s="2"/>
       <c r="S3" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3" t="str">
         <f>F3+I3+L3+O3+R3+U3</f>
         <v>0</v>
       </c>
       <c r="X3" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Z3">
-        <v>585</v>
+        <v>675</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -766,14 +766,14 @@
         <v>1</v>
       </c>
       <c r="T4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4" t="str">
         <f>F4+I4+L4+O4+R4+U4</f>
         <v>0</v>
       </c>
       <c r="X4" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y4">
         <v>11</v>
@@ -793,17 +793,17 @@
         <v>20</v>
       </c>
       <c r="D5" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H5" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="3">
@@ -814,10 +814,10 @@
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N5" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="3">
@@ -838,13 +838,13 @@
         <v>0</v>
       </c>
       <c r="X5" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="Y5">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="Z5">
-        <v>420</v>
+        <v>560</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -865,17 +865,17 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K6" s="4">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="3">
@@ -903,13 +903,13 @@
         <v>0</v>
       </c>
       <c r="X6" s="5">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="Y6">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="Z6">
-        <v>420</v>
+        <v>520</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -937,10 +937,10 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K7" s="4">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="3">
@@ -951,30 +951,30 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q7" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R7" s="2"/>
       <c r="S7" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T7" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W7" t="str">
         <f>F7+I7+L7+O7+R7+U7</f>
         <v>0</v>
       </c>
       <c r="X7" s="5">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="Y7">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Z7">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1016,10 +1016,10 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="3">
@@ -1033,13 +1033,13 @@
         <v>0</v>
       </c>
       <c r="X8" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y8">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="Z8">
-        <v>1040</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -1067,17 +1067,17 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K9" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="3">
@@ -1088,23 +1088,23 @@
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W9" t="str">
         <f>F9+I9+L9+O9+R9+U9</f>
         <v>0</v>
       </c>
       <c r="X9" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Y9">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="Z9">
-        <v>1400</v>
+        <v>1800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>